<commit_message>
Publish Latest checklists 2022-11-18
Updates based on OWASP/wstg@5337d0b
</commit_message>
<xml_diff>
--- a/checklists/checklist.xlsx
+++ b/checklists/checklist.xlsx
@@ -1545,7 +1545,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="66" customHeight="1" s="82">
+    <row r="6" ht="82.5" customHeight="1" s="82">
       <c r="A6" s="19" t="n"/>
       <c r="B6" s="34" t="inlineStr">
         <is>
@@ -1558,7 +1558,8 @@
       </c>
       <c r="D6" s="16" t="inlineStr">
         <is>
-          <t>- Identify what sensitive design and configuration information of the application, system, or organization is exposed directly (on the organization's website) or indirectly (via third-party services).</t>
+          <t>- Identify what sensitive design and configuration information of the application, system, or organization is exposed directly (on the organization's website) or indirectly (via third-party services).
+- New objective.</t>
         </is>
       </c>
       <c r="E6" s="18" t="inlineStr">

</xml_diff>

<commit_message>
Publish Latest checklists 2024-05-22
Updates based on OWASP/wstg@3c41706
</commit_message>
<xml_diff>
--- a/checklists/checklist.xlsx
+++ b/checklists/checklist.xlsx
@@ -1545,7 +1545,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="66" customHeight="1" s="82">
+    <row r="6" ht="82.5" customHeight="1" s="82">
       <c r="A6" s="19" t="n"/>
       <c r="B6" s="34" t="inlineStr">
         <is>
@@ -1558,7 +1558,8 @@
       </c>
       <c r="D6" s="16" t="inlineStr">
         <is>
-          <t>- Identify what sensitive design and configuration information of the application, system, or organization is exposed directly (on the organization's website) or indirectly (via third-party services).</t>
+          <t>- Identify what sensitive design and configuration information of the application, system, or organization is exposed directly (on the organization's website) or indirectly (via third-party services).
+- New objective.</t>
         </is>
       </c>
       <c r="E6" s="18" t="inlineStr">
@@ -4458,7 +4459,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation sqref="E4 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E32 E33 E34 E35 E36 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 E51 E52 E53 E54 E55 E58 E59 E60 E61 E62 E63 E64 E65 E66 E67 E70 E71 E72 E73 E74 E75 E76 E77 E78 E79 E80 E81 E82 E83 E84 E85 E86 E87 E88 E89 E90 E93 E94 E97 E98 E99 E100 E103 E104 E105 E106 E107 E108 E109 E110 E111 E112 E115 E116 E117 E118 E119 E120 E121 E122 E123 E124 E125 E126 E127 E128 E131" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="E4 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E32 E33 E34 E35 E36 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 E51 E52 E53 E54 E55 E58 E59 E60 E61 E62 E63 E64 E65 E66 E67 E70 E71 E72 E73 E74 E75 E76 E77 E78 E79 E80 E81 E82 E83 E84 E85 E86 E87 E88 E89 E90 E93 E94 E97 E98 E99 E100 E103 E104 E105 E106 E107 E108 E109 E110 E111 E112 E115 E116 E117 E118 E119 E120 E121 E122 E123 E124 E125 E126 E127 E128 E131" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Not Started,Pass,Issues,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5386,26 +5387,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="C7:E7"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="C6:E6"/>
     <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C8:E8"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <conditionalFormatting sqref="E20:G20">
     <cfRule type="containsText" priority="1" operator="containsText" dxfId="10" text="critical">
@@ -5424,12 +5425,12 @@
       <formula>NOT(ISERROR(SEARCH(("Note"),(E20))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:E23 B24:B26">
+  <conditionalFormatting sqref="B24:B26 C23:E23">
     <cfRule type="containsText" priority="6" operator="containsText" dxfId="0" text="&lt;">
       <formula>NOT(ISERROR(SEARCH(("&lt;"),(C23))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:E26 B24:B26">
+  <conditionalFormatting sqref="B24:B26 C23:E26">
     <cfRule type="containsText" priority="7" operator="containsText" dxfId="0" text="&lt;">
       <formula>NOT(ISERROR(SEARCH(("&lt;"),(C23))))</formula>
     </cfRule>
@@ -5455,52 +5456,52 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation sqref="H5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="H5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>LossofConfidentiality</formula1>
     </dataValidation>
-    <dataValidation sqref="H7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="H7" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>LossofAvailability</formula1>
     </dataValidation>
-    <dataValidation sqref="H6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="H6" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>LossofIntegrity</formula1>
     </dataValidation>
-    <dataValidation sqref="C13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C13" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>Awareness</formula1>
     </dataValidation>
-    <dataValidation sqref="H13" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="H13" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>NonCompliance</formula1>
     </dataValidation>
-    <dataValidation sqref="H14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="H14" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>PolicyViolation</formula1>
     </dataValidation>
-    <dataValidation sqref="H11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="H11" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>FinancialDamage</formula1>
     </dataValidation>
-    <dataValidation sqref="C11" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C11" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>EasyofDiscovery</formula1>
     </dataValidation>
-    <dataValidation sqref="C6" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C6" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>Motive</formula1>
     </dataValidation>
-    <dataValidation sqref="H8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="H8" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>LossofAccountability</formula1>
     </dataValidation>
-    <dataValidation sqref="C12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C12" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>EaseofExploit</formula1>
     </dataValidation>
-    <dataValidation sqref="C14" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C14" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>IntrusionDetection</formula1>
     </dataValidation>
-    <dataValidation sqref="H12" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="H12" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>ReputationDamage</formula1>
     </dataValidation>
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C5" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>SkillRequired</formula1>
     </dataValidation>
-    <dataValidation sqref="C7" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C7" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>Opportunity</formula1>
     </dataValidation>
-    <dataValidation sqref="C8" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C8" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" type="list">
       <formula1>PopulationSize</formula1>
     </dataValidation>
   </dataValidations>
@@ -5600,7 +5601,7 @@
       </c>
       <c r="B2" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="C2" s="73" t="inlineStr">
@@ -5610,7 +5611,7 @@
       </c>
       <c r="D2" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="E2" s="73" t="inlineStr">
@@ -5620,7 +5621,7 @@
       </c>
       <c r="F2" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="G2" s="73" t="inlineStr">
@@ -5630,7 +5631,7 @@
       </c>
       <c r="H2" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="I2" s="73" t="inlineStr">
@@ -5640,7 +5641,7 @@
       </c>
       <c r="J2" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="K2" s="73" t="inlineStr">
@@ -5650,7 +5651,7 @@
       </c>
       <c r="L2" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="M2" s="73" t="inlineStr">
@@ -5660,7 +5661,7 @@
       </c>
       <c r="N2" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="O2" s="73" t="inlineStr">
@@ -5670,7 +5671,7 @@
       </c>
       <c r="P2" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6081,7 +6082,7 @@
       </c>
       <c r="B11" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="C11" s="73" t="inlineStr">
@@ -6091,7 +6092,7 @@
       </c>
       <c r="D11" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="E11" s="73" t="inlineStr">
@@ -6101,7 +6102,7 @@
       </c>
       <c r="F11" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="G11" s="73" t="inlineStr">
@@ -6111,7 +6112,7 @@
       </c>
       <c r="H11" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="I11" s="73" t="inlineStr">
@@ -6121,7 +6122,7 @@
       </c>
       <c r="J11" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="K11" s="73" t="inlineStr">
@@ -6131,7 +6132,7 @@
       </c>
       <c r="L11" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="M11" s="73" t="inlineStr">
@@ -6141,7 +6142,7 @@
       </c>
       <c r="N11" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="O11" s="73" t="inlineStr">
@@ -6151,7 +6152,7 @@
       </c>
       <c r="P11" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
     </row>

</xml_diff>